<commit_message>
2021/03/09 Start developing multi-threading
</commit_message>
<xml_diff>
--- a/Crawling_Example.xlsx
+++ b/Crawling_Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yilint/Dropbox/Projects/Zillow/Crawl/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YUZHI\Desktop\房地產爬蟲\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E95D7E-BFDA-7444-B2A1-C404623628A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C143EAB-A4B9-4987-98EB-80D6491885BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5000" yWindow="460" windowWidth="28040" windowHeight="17540" xr2:uid="{2AEDFBC9-7DC5-004C-8C6A-2FD3C11C9279}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="4932" firstSheet="1" activeTab="5" xr2:uid="{2AEDFBC9-7DC5-004C-8C6A-2FD3C11C9279}"/>
   </bookViews>
   <sheets>
     <sheet name="Crosswalk" sheetId="3" r:id="rId1"/>
@@ -29,21 +29,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="201">
   <si>
     <t>HouseID</t>
   </si>
@@ -552,105 +543,114 @@
     <t>Market Competition</t>
   </si>
   <si>
+    <t>Average_pending_days</t>
+  </si>
+  <si>
+    <t>Hot_homes_pending_days</t>
+  </si>
+  <si>
+    <t>Average_above_list_price</t>
+  </si>
+  <si>
+    <t>Hot_homes_above_list_prices</t>
+  </si>
+  <si>
+    <t>Nearby Similar Homes (first 6 homes)</t>
+  </si>
+  <si>
+    <t>Redfin_similar_https</t>
+  </si>
+  <si>
+    <t>https://www.redfin.com/CA/Northridge/8800-Etiwanda-Ave-91325/unit-4/home/8177406</t>
+  </si>
+  <si>
+    <t>https://www.redfin.com/CA/Chatsworth/21025-Lemarsh-St-91311/unit-F32/home/5836799</t>
+  </si>
+  <si>
+    <t>https://www.redfin.com/CA/Woodland-Hills/5720-Owensmouth-Ave-91367/unit-157/home/4002425</t>
+  </si>
+  <si>
+    <t>https://www.redfin.com/CA/Tarzana/18135-Burbank-Blvd-91356/unit-3/home/4075518</t>
+  </si>
+  <si>
+    <t>https://www.redfin.com/CA/Reseda/6633-Wilbur-Ave-91335/unit-45/home/3880446</t>
+  </si>
+  <si>
+    <t>https://www.redfin.com/CA/Van-Nuys/7046-De-Celis-Pl-91406/unit-6/home/8151032</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homes/20665152_zpid/</t>
+  </si>
+  <si>
+    <t>Schools</t>
+  </si>
+  <si>
+    <t>GreatSchoolsRating</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Seventh Street Elementary School</t>
+  </si>
+  <si>
+    <t>Everest Value</t>
+  </si>
+  <si>
+    <t>Enadia Technology Enriched Charter School</t>
+  </si>
+  <si>
+    <t>Christopher Columbus Middle School</t>
+  </si>
+  <si>
+    <t>Aspire Pacific Academy</t>
+  </si>
+  <si>
+    <t>Canoga Park Senior High School</t>
+  </si>
+  <si>
+    <t>Independence Continuation School</t>
+  </si>
+  <si>
+    <t>N_students</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>N_reviews</t>
+  </si>
+  <si>
+    <t>Zillow_URL</t>
+  </si>
+  <si>
+    <t>Zillow_Similar_URL</t>
+  </si>
+  <si>
+    <t>Redfin_URL</t>
+  </si>
+  <si>
+    <t>https://www.redfin.com/CA/Monterey-Park/670-Hamlet-Dr-91755/home/6975730</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.redfin.com/CA/Torrance/23302-Marigold-Ave-90502/unit-Y202/home/7670651</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
     <t>Redfin_Compete_Score</t>
-  </si>
-  <si>
-    <t>Average_pending_days</t>
-  </si>
-  <si>
-    <t>Hot_homes_pending_days</t>
-  </si>
-  <si>
-    <t>Average_above_list_price</t>
-  </si>
-  <si>
-    <t>Hot_homes_above_list_prices</t>
-  </si>
-  <si>
-    <t>Nearby Similar Homes (first 6 homes)</t>
-  </si>
-  <si>
-    <t>Redfin_similar_https</t>
-  </si>
-  <si>
-    <t>https://www.redfin.com/CA/Northridge/8800-Etiwanda-Ave-91325/unit-4/home/8177406</t>
-  </si>
-  <si>
-    <t>https://www.redfin.com/CA/Chatsworth/21025-Lemarsh-St-91311/unit-F32/home/5836799</t>
-  </si>
-  <si>
-    <t>https://www.redfin.com/CA/Woodland-Hills/5720-Owensmouth-Ave-91367/unit-157/home/4002425</t>
-  </si>
-  <si>
-    <t>https://www.redfin.com/CA/Tarzana/18135-Burbank-Blvd-91356/unit-3/home/4075518</t>
-  </si>
-  <si>
-    <t>https://www.redfin.com/CA/Reseda/6633-Wilbur-Ave-91335/unit-45/home/3880446</t>
-  </si>
-  <si>
-    <t>https://www.redfin.com/CA/Van-Nuys/7046-De-Celis-Pl-91406/unit-6/home/8151032</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homes/20665152_zpid/</t>
-  </si>
-  <si>
-    <t>Schools</t>
-  </si>
-  <si>
-    <t>GreatSchoolsRating</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Seventh Street Elementary School</t>
-  </si>
-  <si>
-    <t>Everest Value</t>
-  </si>
-  <si>
-    <t>Enadia Technology Enriched Charter School</t>
-  </si>
-  <si>
-    <t>Christopher Columbus Middle School</t>
-  </si>
-  <si>
-    <t>Aspire Pacific Academy</t>
-  </si>
-  <si>
-    <t>Canoga Park Senior High School</t>
-  </si>
-  <si>
-    <t>Independence Continuation School</t>
-  </si>
-  <si>
-    <t>N_students</t>
-  </si>
-  <si>
-    <t>Distance</t>
-  </si>
-  <si>
-    <t>N_reviews</t>
-  </si>
-  <si>
-    <t>Zillow_URL</t>
-  </si>
-  <si>
-    <t>Zillow_Similar_URL</t>
-  </si>
-  <si>
-    <t>Redfin_URL</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -658,27 +658,34 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -811,8 +818,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -828,7 +835,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1126,19 +1133,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4465B078-A04D-8543-B6F8-44F9AE2ABF5D}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.83203125" customWidth="1"/>
-    <col min="5" max="5" width="27.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" customWidth="1"/>
     <col min="7" max="7" width="81.6640625" customWidth="1"/>
-    <col min="8" max="8" width="42.83203125" customWidth="1"/>
+    <col min="8" max="8" width="42.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
@@ -1150,7 +1157,7 @@
       <c r="G1" s="26"/>
       <c r="H1" s="30"/>
     </row>
-    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1170,13 +1177,13 @@
         <v>5</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1202,7 +1209,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1215,14 +1222,14 @@
       <c r="F4">
         <v>91755</v>
       </c>
-      <c r="G4" t="s">
-        <v>16</v>
+      <c r="G4" s="3" t="s">
+        <v>198</v>
       </c>
       <c r="H4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1241,11 +1248,11 @@
       <c r="F5">
         <v>90502</v>
       </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G5" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1268,7 +1275,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1286,10 +1293,14 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" xr:uid="{B0F2DECD-312E-A141-B924-DCB9C3E9D37A}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{F163859E-5BD9-43D9-9281-2F259F2B4555}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{36067C71-C1A2-471B-AFBE-050D3B2F6893}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1301,26 +1312,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="64" customWidth="1"/>
-    <col min="2" max="2" width="125.83203125" customWidth="1"/>
+    <col min="2" max="2" width="125.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="7" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" s="7" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>42</v>
       </c>
@@ -1328,7 +1339,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>42</v>
       </c>
@@ -1336,7 +1347,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>42</v>
       </c>
@@ -1344,7 +1355,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -1352,7 +1363,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -1360,7 +1371,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>42</v>
       </c>
@@ -1368,7 +1379,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>42</v>
       </c>
@@ -1376,7 +1387,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>42</v>
       </c>
@@ -1384,7 +1395,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>42</v>
       </c>
@@ -1393,6 +1404,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1401,26 +1413,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B8103CC-2D22-3249-BE27-C5436F0C26D5}">
   <dimension ref="A1:BA7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="AX2" sqref="AX2:BA2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="7" width="7.83203125" customWidth="1"/>
+    <col min="6" max="7" width="7.77734375" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" customWidth="1"/>
     <col min="10" max="10" width="12.6640625" customWidth="1"/>
     <col min="11" max="15" width="10.6640625" customWidth="1"/>
-    <col min="16" max="37" width="15.1640625" customWidth="1"/>
+    <col min="16" max="37" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>113</v>
       </c>
@@ -1446,9 +1458,9 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:53" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:53" s="10" customFormat="1" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -1592,22 +1604,22 @@
         <v>167</v>
       </c>
       <c r="AW2" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="AX2" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="AY2" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="AX2" s="10" t="s">
+      <c r="AZ2" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="AY2" s="10" t="s">
+      <c r="BA2" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="AZ2" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="BA2" s="10" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>7</v>
       </c>
@@ -1766,7 +1778,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1807,7 +1819,7 @@
       <c r="AJ4" s="5"/>
       <c r="AK4" s="5"/>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1848,7 +1860,7 @@
       <c r="AJ5" s="5"/>
       <c r="AK5" s="5"/>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1889,7 +1901,7 @@
       <c r="AJ6" s="5"/>
       <c r="AK6" s="5"/>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1931,7 +1943,9 @@
       <c r="AK7" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1941,16 +1955,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="74.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" customWidth="1"/>
     <col min="4" max="4" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B1" s="29" t="s">
         <v>78</v>
@@ -1965,7 +1979,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>7</v>
       </c>
@@ -1982,7 +1996,7 @@
         <v>346000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>7</v>
       </c>
@@ -1999,7 +2013,7 @@
         <v>346000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>7</v>
       </c>
@@ -2013,7 +2027,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>7</v>
       </c>
@@ -2027,7 +2041,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>7</v>
       </c>
@@ -2041,7 +2055,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>7</v>
       </c>
@@ -2072,22 +2086,22 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.83203125" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+    <col min="1" max="1" width="36.77734375" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" customWidth="1"/>
     <col min="4" max="4" width="27.6640625" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>86</v>
@@ -2102,7 +2116,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2119,7 +2133,7 @@
         <v>168025</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2136,7 +2150,7 @@
         <v>164731</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2154,7 +2168,7 @@
       </c>
       <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2171,7 +2185,7 @@
         <v>1558335</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2188,7 +2202,7 @@
         <v>155231</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2205,7 +2219,7 @@
         <v>830000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2222,7 +2236,7 @@
         <v>69000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -2239,7 +2253,7 @@
         <v>63000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -2256,37 +2270,37 @@
         <v>67100</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="22"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -2317,150 +2331,151 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="88.6640625" customWidth="1"/>
-    <col min="2" max="2" width="50.83203125" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+    <col min="2" max="2" width="50.77734375" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" customWidth="1"/>
     <col min="4" max="4" width="27.6640625" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
       <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="22"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{A63D8EB4-DFCD-9348-AFA7-41EB906A0A7E}"/>
     <hyperlink ref="A4" r:id="rId2" xr:uid="{DBE9C9C4-C9E5-C04F-84F6-808D58FE0A58}"/>
@@ -2477,51 +2492,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293E71D9-0E40-7F48-A9E8-7EA429E44565}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="88.6640625" customWidth="1"/>
     <col min="2" max="2" width="36.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>184</v>
-      </c>
       <c r="D2" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="F2" s="29" t="s">
         <v>193</v>
       </c>
-      <c r="E2" s="29" t="s">
-        <v>195</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C3" s="22">
         <v>4</v>
@@ -2536,12 +2551,12 @@
         <v>36.700000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C4" s="22">
         <v>6</v>
@@ -2554,12 +2569,12 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C5" s="22">
         <v>6</v>
@@ -2575,12 +2590,12 @@
       </c>
       <c r="G5" s="22"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C6" s="22">
         <v>3</v>
@@ -2595,12 +2610,12 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C7" s="22">
         <v>4</v>
@@ -2615,12 +2630,12 @@
         <v>26.6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C8" s="22">
         <v>3</v>
@@ -2635,12 +2650,12 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="22">
@@ -2653,56 +2668,56 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="22"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -2710,6 +2725,7 @@
       <c r="F17" s="22"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{3CAEF78B-BFD4-F64D-B09A-93CF357D41E7}"/>
     <hyperlink ref="A4" r:id="rId2" xr:uid="{49FC3447-6431-2347-B3B7-223CBB348907}"/>
@@ -2731,25 +2747,25 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.5" customWidth="1"/>
+    <col min="1" max="1" width="42.44140625" customWidth="1"/>
     <col min="2" max="2" width="5.33203125" customWidth="1"/>
     <col min="3" max="3" width="6.33203125" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" customWidth="1"/>
     <col min="10" max="10" width="12.33203125" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="7"/>
-    <col min="20" max="20" width="14.1640625" customWidth="1"/>
-    <col min="28" max="29" width="9.1640625" customWidth="1"/>
+    <col min="11" max="11" width="10.77734375" style="7"/>
+    <col min="20" max="20" width="14.109375" customWidth="1"/>
+    <col min="28" max="29" width="9.109375" customWidth="1"/>
     <col min="30" max="30" width="10" customWidth="1"/>
-    <col min="31" max="34" width="10.1640625" customWidth="1"/>
+    <col min="31" max="34" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" ht="32.4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>113</v>
       </c>
@@ -2769,9 +2785,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" s="10" customFormat="1" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>44</v>
@@ -2879,7 +2895,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:36" s="7" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>42</v>
       </c>
@@ -2990,6 +3006,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3002,20 +3019,20 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46.6640625" customWidth="1"/>
-    <col min="5" max="5" width="29.5" style="11" customWidth="1"/>
+    <col min="5" max="5" width="29.44140625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>78</v>
@@ -3030,7 +3047,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>42</v>
       </c>
@@ -3048,7 +3065,7 @@
       </c>
       <c r="F3" s="13"/>
     </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>42</v>
       </c>
@@ -3065,7 +3082,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>42</v>
       </c>
@@ -3082,7 +3099,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -3099,7 +3116,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3117,6 +3134,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3129,22 +3147,22 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46.6640625" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="29.5" style="11" customWidth="1"/>
+    <col min="5" max="5" width="29.44140625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>86</v>
@@ -3157,7 +3175,7 @@
       </c>
       <c r="E2" s="15"/>
     </row>
-    <row r="3" spans="1:6" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>42</v>
       </c>
@@ -3173,7 +3191,7 @@
       <c r="E3" s="11"/>
       <c r="F3" s="13"/>
     </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>42</v>
       </c>
@@ -3187,7 +3205,7 @@
         <v>372773</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>42</v>
       </c>
@@ -3201,7 +3219,7 @@
         <v>365464</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -3215,7 +3233,7 @@
         <v>358299</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3229,7 +3247,7 @@
         <v>351275</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>42</v>
       </c>
@@ -3243,7 +3261,7 @@
         <v>390000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>42</v>
       </c>
@@ -3257,7 +3275,7 @@
         <v>325000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>42</v>
       </c>
@@ -3268,7 +3286,7 @@
         <v>247000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>42</v>
       </c>
@@ -3279,7 +3297,7 @@
         <v>265000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>42</v>
       </c>
@@ -3290,16 +3308,17 @@
         <v>265000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="18"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="18"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="18"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>